<commit_message>
just need to resize image and then were good
</commit_message>
<xml_diff>
--- a/Excel Files/Access Permission Table.xlsx
+++ b/Excel Files/Access Permission Table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B729DE-1CA6-479A-8306-ABE1EB4A5340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4070" yWindow="4070" windowWidth="21600" windowHeight="11390"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
   <si>
     <t>Appliances</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Convenience Store</t>
   </si>
   <si>
-    <t>Banner</t>
-  </si>
-  <si>
     <t>Business Unit</t>
   </si>
   <si>
@@ -61,12 +59,24 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Yap </t>
+  </si>
+  <si>
+    <t>stephen.yap@robinsonsretail.ph</t>
+  </si>
+  <si>
+    <t>Josemaria Catanghal</t>
+  </si>
+  <si>
+    <t>Josemaria.Catanghal@robinsonsretail.com.ph</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,86 +441,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{738C6937-8CAA-4A12-A0AD-436975E09EE4}"/>
+    <hyperlink ref="C3:C11" r:id="rId2" display="stephen.yap@robinsonsretail.ph" xr:uid="{B4FD155A-1CD4-4432-A25C-664C7F9FD424}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed sheet name of perm table excel
</commit_message>
<xml_diff>
--- a/Excel Files/Access Permission Table.xlsx
+++ b/Excel Files/Access Permission Table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9372274-D130-4877-AAA0-7BE86AE02EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A0DEDA-0ACC-4891-A8E1-B1EED1471CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Permissions List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -669,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
       <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Data Validation for Access Permission and All Data Excel
</commit_message>
<xml_diff>
--- a/Excel Files/Access Permission Table.xlsx
+++ b/Excel Files/Access Permission Table.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CA.Intern\Desktop\PMO-Dashboard\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A0DEDA-0ACC-4891-A8E1-B1EED1471CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions List" sheetId="1" r:id="rId1"/>
+    <sheet name="All Business Units" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="92">
   <si>
     <t>Appliances</t>
   </si>
@@ -301,8 +301,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +322,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -359,12 +364,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,22 +674,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="2"/>
+    <col min="4" max="4" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -692,7 +700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -703,7 +711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -714,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -725,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -736,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -747,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -758,7 +766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -769,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -780,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -791,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -802,7 +810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -813,7 +821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -824,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -835,7 +843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -846,7 +854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -857,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -868,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -879,7 +887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -890,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -901,7 +909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -912,7 +920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -923,7 +931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -934,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -945,7 +953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -956,7 +964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -967,7 +975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -978,7 +986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -989,7 +997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1000,7 +1008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1066,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1110,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1132,7 +1140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1154,7 +1162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1176,7 +1184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1187,7 +1195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +1206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1239,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1253,7 +1261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1341,7 +1349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1385,7 +1393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1396,7 +1404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1426,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1448,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -1462,7 +1470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1492,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -1495,7 +1503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -1517,7 +1525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>9</v>
       </c>
@@ -1528,7 +1536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -1572,7 +1580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -1583,7 +1591,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -1594,7 +1602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -1616,7 +1624,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -1627,7 +1635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1646,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1657,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -1660,7 +1668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -1671,7 +1679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -1682,7 +1690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -1693,7 +1701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1712,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -1715,7 +1723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -1726,7 +1734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -1737,7 +1745,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -1803,7 +1811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -1825,7 +1833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -1836,7 +1844,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -1847,7 +1855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -1858,7 +1866,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -1891,7 +1899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -1902,7 +1910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -1913,7 +1921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -1924,7 +1932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -1935,7 +1943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -1957,7 +1965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -1968,7 +1976,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1987,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -1990,7 +1998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -2001,7 +2009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>7</v>
       </c>
@@ -2012,7 +2020,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -2023,7 +2031,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -2034,7 +2042,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>2</v>
       </c>
@@ -2045,7 +2053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1</v>
       </c>
@@ -2056,7 +2064,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -2067,7 +2075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -2078,7 +2086,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -2089,7 +2097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -2100,7 +2108,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -2111,7 +2119,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>7</v>
       </c>
@@ -2122,7 +2130,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -2133,7 +2141,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>3</v>
       </c>
@@ -2144,7 +2152,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -2155,7 +2163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2174,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -2177,7 +2185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -2188,7 +2196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -2199,7 +2207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -2210,7 +2218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -2232,7 +2240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>4</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2262,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -2265,7 +2273,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1</v>
       </c>
@@ -2276,7 +2284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -2287,7 +2295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -2298,7 +2306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -2320,7 +2328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -2331,7 +2339,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>7</v>
       </c>
@@ -2342,7 +2350,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>4</v>
       </c>
@@ -2353,7 +2361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2372,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -2375,7 +2383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -2386,7 +2394,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -2397,7 +2405,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -2408,7 +2416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>5</v>
       </c>
@@ -2430,7 +2438,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>6</v>
       </c>
@@ -2441,7 +2449,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>7</v>
       </c>
@@ -2452,7 +2460,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>4</v>
       </c>
@@ -2463,7 +2471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2482,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -2485,7 +2493,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>1</v>
       </c>
@@ -2496,7 +2504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -2507,7 +2515,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -2518,7 +2526,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>5</v>
       </c>
@@ -2540,7 +2548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>6</v>
       </c>
@@ -2551,7 +2559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>7</v>
       </c>
@@ -2562,7 +2570,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>4</v>
       </c>
@@ -2573,7 +2581,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>3</v>
       </c>
@@ -2584,7 +2592,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -2595,7 +2603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>1</v>
       </c>
@@ -2606,7 +2614,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -2617,7 +2625,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -2628,7 +2636,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -2639,7 +2647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2658,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>6</v>
       </c>
@@ -2661,7 +2669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>4</v>
       </c>
@@ -2683,7 +2691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>3</v>
       </c>
@@ -2694,7 +2702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -2705,7 +2713,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1</v>
       </c>
@@ -2716,7 +2724,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>8</v>
       </c>
@@ -2727,7 +2735,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -2738,7 +2746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>5</v>
       </c>
@@ -2760,7 +2768,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>6</v>
       </c>
@@ -2771,7 +2779,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>7</v>
       </c>
@@ -2782,7 +2790,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2801,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>4</v>
       </c>
@@ -2804,7 +2812,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>4</v>
       </c>
@@ -2815,7 +2823,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>4</v>
       </c>
@@ -2826,7 +2834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>3</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>2</v>
       </c>
@@ -2848,7 +2856,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -2859,7 +2867,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>1</v>
       </c>
@@ -2870,7 +2878,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>8</v>
       </c>
@@ -2881,7 +2889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -2889,7 +2897,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -2897,7 +2905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>9</v>
       </c>
@@ -2905,7 +2913,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -2916,7 +2924,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -2927,7 +2935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>5</v>
       </c>
@@ -2938,7 +2946,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>5</v>
       </c>
@@ -2949,7 +2957,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>6</v>
       </c>
@@ -2960,7 +2968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>6</v>
       </c>
@@ -2971,7 +2979,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>6</v>
       </c>
@@ -2982,7 +2990,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>6</v>
       </c>
@@ -2993,7 +3001,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -3004,7 +3012,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>7</v>
       </c>
@@ -3015,7 +3023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>7</v>
       </c>
@@ -3026,7 +3034,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>7</v>
       </c>
@@ -3037,7 +3045,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3056,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -3059,7 +3067,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>7</v>
       </c>
@@ -3070,7 +3078,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>7</v>
       </c>
@@ -3081,7 +3089,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>7</v>
       </c>
@@ -3095,5 +3103,90 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'All Business Units'!$A$2:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>